<commit_message>
fix test no coupling
</commit_message>
<xml_diff>
--- a/tests/test_cases/functional_cases/case_no_coupling/testInputs/TestVec.xlsx
+++ b/tests/test_cases/functional_cases/case_no_coupling/testInputs/TestVec.xlsx
@@ -94,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -117,13 +117,7 @@
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,9 +335,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="4" width="12.63"/>
     <col customWidth="1" min="5" max="5" width="19.13"/>
-    <col customWidth="1" min="6" max="6" width="12.63"/>
     <col customWidth="1" min="9" max="9" width="20.0"/>
   </cols>
   <sheetData>
@@ -404,12 +396,12 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G3" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="H3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="7">
         <v>0.0</v>
       </c>
       <c r="I3" s="6"/>
@@ -429,12 +421,12 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="H4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="7">
         <v>0.0</v>
       </c>
       <c r="I4" s="6"/>
@@ -454,12 +446,12 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G5" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="H5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="7">
         <v>0.0</v>
       </c>
       <c r="I5" s="6"/>
@@ -479,12 +471,12 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="H6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H6" s="7">
         <v>0.0</v>
       </c>
       <c r="I6" s="6"/>
@@ -504,12 +496,12 @@
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="H7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="7">
         <v>0.0</v>
       </c>
       <c r="I7" s="6"/>
@@ -529,12 +521,12 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G8" s="7">
-        <v>6.0</v>
-      </c>
-      <c r="H8" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="7">
         <v>0.0</v>
       </c>
       <c r="I8" s="6"/>
@@ -554,12 +546,12 @@
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="7">
-        <v>4204391.0</v>
+        <v>0.0</v>
       </c>
       <c r="G9" s="7">
-        <v>7.0</v>
-      </c>
-      <c r="H9" s="9">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="7">
         <v>0.0</v>
       </c>
       <c r="I9" s="6"/>

</xml_diff>